<commit_message>
smart cut excel format
</commit_message>
<xml_diff>
--- a/VralumGlassWeb/wwwroot/storage/SmartCutCalculation.xlsx
+++ b/VralumGlassWeb/wwwroot/storage/SmartCutCalculation.xlsx
@@ -12,18 +12,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
-  <si>
-    <t xml:space="preserve">18.12.2019 09:21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plank Length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Snippet [Floor/Apartment]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+  <si>
+    <t xml:space="preserve">19.12.2019 08:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6300 X 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Planks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snippets [Floor/Apartment]</t>
   </si>
   <si>
     <t xml:space="preserve">Waste</t>
@@ -314,40 +320,27 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6"/>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5">
-        <v>150</v>
-      </c>
     </row>
     <row r="8">
-      <c r="B8" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="C8" s="5">
-        <v>25</v>
       </c>
     </row>
     <row r="9">
@@ -355,60 +348,60 @@
         <v>8</v>
       </c>
       <c r="C9" s="5">
-        <v>165</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="5">
-        <v>605</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="5">
-        <v>180</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="5">
-        <v>70</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="5">
-        <v>100</v>
+        <v>605</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="5">
-        <v>100</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="5">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="5">
         <v>100</v>
@@ -416,7 +409,7 @@
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="5">
         <v>100</v>
@@ -424,7 +417,7 @@
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="5">
         <v>100</v>
@@ -432,71 +425,71 @@
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="5">
-        <v>170</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="5">
-        <v>170</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="5">
-        <v>130</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="5">
-        <v>130</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="5">
-        <v>130</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="5">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="5">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="5">
-        <v>170</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="5">
         <v>170</v>
@@ -504,84 +497,84 @@
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="5">
-        <v>500</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="5">
-        <v>340</v>
+        <v>170</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C30" s="5">
-        <v>340</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C31" s="5">
-        <v>340</v>
+        <v>500</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C32" s="5">
         <v>340</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="s">
-        <v>32</v>
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="5">
+        <v>340</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C34" s="5">
-        <v>0</v>
+        <v>340</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="5">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="C35" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" s="5">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C38" s="5">
         <v>0</v>
@@ -589,23 +582,23 @@
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C40" s="5">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" s="5">
         <v>0</v>
@@ -613,31 +606,31 @@
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C42" s="5">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43" s="5">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C44" s="5">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C45" s="5">
         <v>20</v>
@@ -645,15 +638,15 @@
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C46" s="5">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C47" s="5">
         <v>20</v>
@@ -661,80 +654,104 @@
     </row>
     <row r="48">
       <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="5">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="4" t="s">
-        <v>48</v>
+      <c r="C49" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C50" s="5">
-        <v>725</v>
+        <v>20</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C51" s="5">
-        <v>840</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="B52" t="s">
-        <v>51</v>
-      </c>
-      <c r="C52" s="5">
-        <v>30</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C53" s="5">
-        <v>100</v>
+        <v>725</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C54" s="5">
-        <v>40</v>
+        <v>840</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C55" s="5">
-        <v>340</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
+        <v>54</v>
+      </c>
+      <c r="C56" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="s">
         <v>55</v>
       </c>
-      <c r="C56" s="5">
+      <c r="C57" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+      <c r="C58" s="5">
         <v>340</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3" t="s">
+    <row r="59">
+      <c r="B59" t="s">
         <v>57</v>
+      </c>
+      <c r="C59" s="5">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>